<commit_message>
integration test OK, pytest-cov > 80%
</commit_message>
<xml_diff>
--- a/mission/schema_base_de_donnee_P11.xlsx
+++ b/mission/schema_base_de_donnee_P11.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nidal\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nidal\Desktop\OC_P11_GUDLFT_LOCAL\mission\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -776,7 +776,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -851,15 +851,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick">
-        <color theme="8"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color theme="8"/>
       </left>
@@ -873,26 +864,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color rgb="FF92D050"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF92D050"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color rgb="FF92D050"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thick">
         <color rgb="FF92D050"/>
@@ -901,15 +872,6 @@
         <color rgb="FF92D050"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color rgb="FF92D050"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -942,15 +904,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color theme="5"/>
       </left>
@@ -963,11 +916,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF92D050"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF92D050"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -993,42 +959,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1039,6 +990,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1321,221 +1275,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J26"/>
+  <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="54" style="1" customWidth="1"/>
-    <col min="3" max="5" width="11.42578125" style="1"/>
-    <col min="6" max="6" width="63.140625" style="1" customWidth="1"/>
-    <col min="7" max="9" width="11.42578125" style="1"/>
-    <col min="10" max="10" width="63.140625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="1"/>
+    <col min="3" max="4" width="11.42578125" style="1"/>
+    <col min="5" max="5" width="63.140625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" style="1"/>
+    <col min="8" max="8" width="63.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" ht="21.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="4"/>
+      <c r="E2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="11" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="20"/>
+      <c r="H3" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="16" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="5" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="6" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="E6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="17" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="H7" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="8" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="14"/>
     </row>
-    <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="E11" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="12" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="E12" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="13" spans="2:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="E13" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="7"/>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="2:10" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="7"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="15" t="s">
-        <v>19</v>
-      </c>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="2:10" ht="67.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="3:10" ht="31.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" s="14"/>
-      <c r="J17" s="21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="3:10" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="3:10" ht="61.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="3:10" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="17"/>
-      <c r="J20" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G21" s="4"/>
-      <c r="H21" s="17"/>
-    </row>
-    <row r="22" spans="3:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
-    </row>
-    <row r="23" spans="3:10" ht="31.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F23" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="3:10" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="F24" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="3:10" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="F25" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="3:10" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F26" s="3" t="s">
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>